<commit_message>
updated ReadIn in ActorDTO
</commit_message>
<xml_diff>
--- a/Mediathek/src/main/resources/csv/Customer.xlsx
+++ b/Mediathek/src/main/resources/csv/Customer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Schule\DBI\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Schule\DBI\DBIJPA4Mediathek\Mediathek\src\main\resources\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -336,37 +336,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>55.81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>22.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>33.229999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>45.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
+      </c>
+      <c r="B5">
+        <v>90.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>